<commit_message>
Built the input module for users to enter word searches
</commit_message>
<xml_diff>
--- a/zipcodes.xlsx
+++ b/zipcodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Software\gnarfle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42D4DAD-E982-4989-9DD6-BB351A0E3410}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD4DF2C-C8F1-45DF-BA54-9649DCE80EE4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>zip_code</t>
   </si>
@@ -106,13 +106,25 @@
   </si>
   <si>
     <t>King of Prussia</t>
+  </si>
+  <si>
+    <t>Roswell, GA</t>
+  </si>
+  <si>
+    <t>Baltimore, MD</t>
+  </si>
+  <si>
+    <t>Orlando, FL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,6 +258,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -589,9 +607,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -947,15 +967,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -974,107 +994,107 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>19406</v>
+        <v>10001</v>
       </c>
       <c r="B2" t="str">
         <f>TEXT(A2,"#####")</f>
-        <v>19406</v>
+        <v>10001</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>10001</v>
+        <v>90021</v>
       </c>
       <c r="B3" t="str">
         <f>TEXT(A3,"#####")</f>
-        <v>10001</v>
+        <v>90021</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>90021</v>
+        <v>60605</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" ref="B4:B22" si="0">TEXT(A4,"#####")</f>
-        <v>90021</v>
+        <f>TEXT(A4,"#####")</f>
+        <v>60605</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>60605</v>
+        <v>75202</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>60605</v>
+        <f>TEXT(A5,"#####")</f>
+        <v>75202</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>75202</v>
+        <v>77002</v>
       </c>
       <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>75202</v>
+        <f>TEXT(A6,"#####")</f>
+        <v>77002</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>77002</v>
+        <v>20004</v>
       </c>
       <c r="B7" t="str">
-        <f t="shared" si="0"/>
-        <v>77002</v>
+        <f>TEXT(A7,"#####")</f>
+        <v>20004</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="D7" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>20004</v>
+        <v>33131</v>
       </c>
       <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>20004</v>
+        <f>TEXT(A8,"#####")</f>
+        <v>33131</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="D8" s="2">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1082,213 +1102,258 @@
         <v>19102</v>
       </c>
       <c r="B9" t="str">
-        <f t="shared" si="0"/>
+        <f>TEXT(A9,"#####")</f>
         <v>19102</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="D9">
-        <v>0</v>
+      <c r="D9" s="2">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>30303</v>
+        <v>19406</v>
       </c>
       <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>30303</v>
+        <f>TEXT(A10,"#####")</f>
+        <v>19406</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10">
-        <v>9</v>
+        <v>25</v>
+      </c>
+      <c r="D10" s="2">
+        <v>8.1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>33131</v>
+        <v>30303</v>
       </c>
       <c r="B11" t="str">
-        <f t="shared" si="0"/>
-        <v>33131</v>
+        <f>TEXT(A11,"#####")</f>
+        <v>30303</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="D11" s="2">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>15219</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>30076</v>
+      </c>
+      <c r="B12" t="str">
+        <f>TEXT(A12,"#####")</f>
+        <v>30076</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12">
-        <v>10</v>
+        <v>26</v>
+      </c>
+      <c r="D12" s="2">
+        <v>9.1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>85003</v>
-      </c>
-      <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v>85003</v>
+        <v>15219</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="D13" s="2">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>94111</v>
+        <v>85003</v>
       </c>
       <c r="B14" t="str">
-        <f t="shared" si="0"/>
-        <v>94111</v>
+        <f>TEXT(A14,"#####")</f>
+        <v>85003</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="D14" s="2">
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>92501</v>
+        <v>94111</v>
       </c>
       <c r="B15" t="str">
-        <f t="shared" si="0"/>
-        <v>92501</v>
+        <f>TEXT(A15,"#####")</f>
+        <v>94111</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="D15" s="2">
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>48226</v>
+        <v>92501</v>
       </c>
       <c r="B16" t="str">
-        <f t="shared" si="0"/>
-        <v>48226</v>
+        <f>TEXT(A16,"#####")</f>
+        <v>92501</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="D16" s="2">
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>98104</v>
+        <v>48226</v>
       </c>
       <c r="B17" t="str">
-        <f t="shared" si="0"/>
-        <v>98104</v>
+        <f>TEXT(A17,"#####")</f>
+        <v>48226</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="D17" s="2">
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>55402</v>
+        <v>98104</v>
       </c>
       <c r="B18" t="str">
-        <f t="shared" si="0"/>
-        <v>55402</v>
+        <f>TEXT(A18,"#####")</f>
+        <v>98104</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="D18" s="2">
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>92101</v>
+        <v>55402</v>
       </c>
       <c r="B19" t="str">
-        <f t="shared" si="0"/>
-        <v>92101</v>
+        <f>TEXT(A19,"#####")</f>
+        <v>55402</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="D19" s="2">
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>33602</v>
+        <v>92101</v>
       </c>
       <c r="B20" t="str">
-        <f t="shared" si="0"/>
-        <v>33602</v>
+        <f>TEXT(A20,"#####")</f>
+        <v>92101</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="D20" s="2">
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>80204</v>
+        <v>33602</v>
       </c>
       <c r="B21" t="str">
-        <f t="shared" si="0"/>
-        <v>80204</v>
+        <f>TEXT(A21,"#####")</f>
+        <v>33602</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="D21" s="2">
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
+        <v>80204</v>
+      </c>
+      <c r="B22" t="str">
+        <f>TEXT(A22,"#####")</f>
+        <v>80204</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
         <v>63101</v>
       </c>
-      <c r="B22" t="str">
-        <f t="shared" si="0"/>
+      <c r="B23" t="str">
+        <f>TEXT(A23,"#####")</f>
         <v>63101</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>24</v>
       </c>
-      <c r="D22">
+      <c r="D23" s="2">
         <v>20</v>
       </c>
     </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>21202</v>
+      </c>
+      <c r="B24" t="str">
+        <f>TEXT(A24,"#####")</f>
+        <v>21202</v>
+      </c>
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>32801</v>
+      </c>
+      <c r="B25" t="str">
+        <f>TEXT(A25,"#####")</f>
+        <v>32801</v>
+      </c>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="2">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A63">
-    <sortCondition ref="A11:A63"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D23">
+    <sortCondition ref="D2:D23"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>